<commit_message>
it's now more robust
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\UiTests\UiTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\uiTesting\UiTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,55 +557,106 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="1">
+        <v>0.92361111111111116</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="1">
+        <v>0.92361111111111116</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="1">
+        <v>0.92361111111111116</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="1">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.97222222222222221</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>7.6388888888888895E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
as stable as it needs to be
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\uiTesting\UiTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\UiTests\UiTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>2GB Ram server</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>vm1</t>
   </si>
@@ -93,6 +90,12 @@
   </si>
   <si>
     <t>restart</t>
+  </si>
+  <si>
+    <t>2GB Ram server vm</t>
+  </si>
+  <si>
+    <t>FEC 2GB 1.99GHz quad</t>
   </si>
 </sst>
 </file>
@@ -128,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,35 +449,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0.55138888888888882</v>
@@ -481,7 +486,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>0.56874999999999998</v>
@@ -489,7 +494,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>0.58402777777777781</v>
@@ -503,7 +508,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>0.6020833333333333</v>
@@ -511,7 +516,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>0.6020833333333333</v>
@@ -528,7 +533,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>0.65138888888888891</v>
@@ -536,7 +541,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>0.65138888888888891</v>
@@ -544,7 +549,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>0.65138888888888891</v>
@@ -555,7 +560,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>0.92361111111111116</v>
@@ -563,7 +568,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>0.92361111111111116</v>
@@ -571,7 +576,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>0.92361111111111116</v>
@@ -579,7 +584,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>0.92361111111111116</v>
@@ -596,42 +601,42 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>7.1527777777777787E-2</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>42804.071527777778</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>7.1527777777777787E-2</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>42804.071527777778</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>7.1527777777777787E-2</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>42804.071527777778</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>7.1527777777777787E-2</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>42804.071527777778</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>7.1527777777777787E-2</v>
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>42804.071527777778</v>
       </c>
       <c r="C18" s="1">
         <v>7.6388888888888895E-2</v>
@@ -639,10 +644,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>7.1527777777777787E-2</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>42804.071527777778</v>
       </c>
       <c r="C19" s="1">
         <v>7.6388888888888895E-2</v>
@@ -650,16 +655,283 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>7.1527777777777787E-2</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>42804.071527777778</v>
       </c>
       <c r="C20" s="1">
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>42804.40625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2">
+        <v>42804.418055555558</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2">
+        <v>42804.432638888888</v>
+      </c>
+      <c r="C25" s="2">
+        <v>42804.448611111111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2">
+        <v>42804.463194444441</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="2">
+        <v>42804.463194444441</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2">
+        <v>42804.478472222225</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.48402777777777778</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2">
+        <v>42804.478472222225</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.48402777777777778</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2">
+        <v>42804.478472222225</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.48402777777777778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2">
+        <v>42804.520138888889</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2">
+        <v>42804.520138888889</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2">
+        <v>42804.520138888889</v>
+      </c>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="2">
+        <v>42804.520138888889</v>
+      </c>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2">
+        <v>42804.520138888889</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="2">
+        <v>42804.529861111114</v>
+      </c>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="2">
+        <v>42804.529861111114</v>
+      </c>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="2">
+        <v>42804.529861111114</v>
+      </c>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the testplan doc with todays tests?
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FirstTests" sheetId="1" r:id="rId1"/>
+    <sheet name="CleanDatabaseTests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="41">
   <si>
     <t>vm1</t>
   </si>
@@ -114,6 +115,39 @@
   </si>
   <si>
     <t xml:space="preserve">crashed some time over the weekend. </t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>8GB Ram server 2.4 quad vm 1 pos</t>
+  </si>
+  <si>
+    <t>8GB Ram server 2.4 quad vm 3 pos</t>
+  </si>
+  <si>
+    <t>2GB Ram vm 1 pos</t>
+  </si>
+  <si>
+    <t>4GB FEC 1 pos</t>
+  </si>
+  <si>
+    <t>VM 8GB 2.4GHz quad 5pos</t>
+  </si>
+  <si>
+    <t>2GB Ram vm 2 pos</t>
+  </si>
+  <si>
+    <t>4GB FEC 2 pos</t>
+  </si>
+  <si>
+    <t>VM 8GB 2.4GHz quad 8pos</t>
+  </si>
+  <si>
+    <t>2GB Ram vm 3 pos</t>
+  </si>
+  <si>
+    <t>4GB FEC 3 pos</t>
   </si>
 </sst>
 </file>
@@ -469,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,4 +1434,400 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>42809.444444444445</v>
+      </c>
+      <c r="C2" s="2">
+        <v>42809.491666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42809.494444444441</v>
+      </c>
+      <c r="C5" s="2">
+        <v>42809.537499999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42809.494444444441</v>
+      </c>
+      <c r="C6" s="2">
+        <v>42809.537499999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>42809.494444444441</v>
+      </c>
+      <c r="C7" s="2">
+        <v>42809.537499999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>42809.504166666666</v>
+      </c>
+      <c r="C11" s="2">
+        <v>42809.552083333336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>42809.502083333333</v>
+      </c>
+      <c r="C14" s="2">
+        <v>42809.552083333336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>42809.540277777778</v>
+      </c>
+      <c r="C17" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2">
+        <v>42809.540277777778</v>
+      </c>
+      <c r="C18" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2">
+        <v>42809.540277777778</v>
+      </c>
+      <c r="C19" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2">
+        <v>42809.540277777778</v>
+      </c>
+      <c r="C20" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2">
+        <v>42809.540277777778</v>
+      </c>
+      <c r="C21" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>42809.556250000001</v>
+      </c>
+      <c r="C24" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2">
+        <v>42809.556250000001</v>
+      </c>
+      <c r="C25" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2">
+        <v>42809.556944444441</v>
+      </c>
+      <c r="C28" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="2">
+        <v>42809.556944444441</v>
+      </c>
+      <c r="C29" s="2">
+        <v>42809.606249999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C32" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C33" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C34" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C35" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C36" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C37" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C38" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="2">
+        <v>42809.617361111108</v>
+      </c>
+      <c r="C39" s="2">
+        <v>42809.669444444444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="2">
+        <v>42809.626388888886</v>
+      </c>
+      <c r="C42" s="2">
+        <v>42809.677083333336</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="2">
+        <v>42809.626388888886</v>
+      </c>
+      <c r="C43" s="2">
+        <v>42809.677083333336</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="2">
+        <v>42809.626388888886</v>
+      </c>
+      <c r="C44" s="2">
+        <v>42809.677083333336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2">
+        <v>42809.623611111114</v>
+      </c>
+      <c r="C47" s="2">
+        <v>42809.677083333336</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="2">
+        <v>42809.623611111114</v>
+      </c>
+      <c r="C48" s="2">
+        <v>42809.677083333336</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="2">
+        <v>42809.623611111114</v>
+      </c>
+      <c r="C49" s="2">
+        <v>42809.677083333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added trace log files
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="61">
   <si>
     <t>vm1</t>
   </si>
@@ -148,6 +148,66 @@
   </si>
   <si>
     <t>4GB FEC 3 pos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test failed too slow. </t>
+  </si>
+  <si>
+    <t>VM 8GB 2.4GHz quad 9pos</t>
+  </si>
+  <si>
+    <t>VM 8GB 2.4GHz quad 1pos database size</t>
+  </si>
+  <si>
+    <t>2GB Ram vm 1pos database size</t>
+  </si>
+  <si>
+    <t>4GB FEC 1pos database size</t>
+  </si>
+  <si>
+    <t>database size</t>
+  </si>
+  <si>
+    <t>measure time</t>
+  </si>
+  <si>
+    <t>log file size</t>
+  </si>
+  <si>
+    <t>65.23MB</t>
+  </si>
+  <si>
+    <t>1024KB</t>
+  </si>
+  <si>
+    <t>32.25MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stopped for adding records. </t>
+  </si>
+  <si>
+    <t>65.25MB</t>
+  </si>
+  <si>
+    <t>59.25MB</t>
+  </si>
+  <si>
+    <t>110.25MB</t>
+  </si>
+  <si>
+    <t>99.25MB</t>
+  </si>
+  <si>
+    <t>284.25MB</t>
+  </si>
+  <si>
+    <t>484.25MB</t>
+  </si>
+  <si>
+    <t>161.25MB</t>
+  </si>
+  <si>
+    <t>147.25MB</t>
   </si>
 </sst>
 </file>
@@ -1438,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,6 +1509,20 @@
     <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="26.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1826,6 +1900,371 @@
         <v>42809.677083333336</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="2">
+        <v>42810.469444444447</v>
+      </c>
+      <c r="C52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" s="2">
+        <v>42810.469444444447</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>43</v>
+      </c>
+      <c r="C75" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G75" t="s">
+        <v>47</v>
+      </c>
+      <c r="H75" t="s">
+        <v>46</v>
+      </c>
+      <c r="I75" t="s">
+        <v>48</v>
+      </c>
+      <c r="J75" t="s">
+        <v>52</v>
+      </c>
+      <c r="K75" t="s">
+        <v>47</v>
+      </c>
+      <c r="L75" t="s">
+        <v>46</v>
+      </c>
+      <c r="M75" t="s">
+        <v>48</v>
+      </c>
+      <c r="N75" t="s">
+        <v>52</v>
+      </c>
+      <c r="O75" t="s">
+        <v>47</v>
+      </c>
+      <c r="P75" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>48</v>
+      </c>
+      <c r="R75" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="2">
+        <v>42814.367361111108</v>
+      </c>
+      <c r="D76" t="s">
+        <v>49</v>
+      </c>
+      <c r="E76" t="s">
+        <v>50</v>
+      </c>
+      <c r="F76" s="2">
+        <v>42814.583333333336</v>
+      </c>
+      <c r="G76" s="2">
+        <v>42815.555555555555</v>
+      </c>
+      <c r="H76" t="s">
+        <v>55</v>
+      </c>
+      <c r="I76" t="s">
+        <v>50</v>
+      </c>
+      <c r="J76" s="2">
+        <v>42815.677777777775</v>
+      </c>
+      <c r="K76" s="2">
+        <v>42816.388888888891</v>
+      </c>
+      <c r="L76" t="s">
+        <v>57</v>
+      </c>
+      <c r="M76" t="s">
+        <v>50</v>
+      </c>
+      <c r="N76" s="2">
+        <v>42816.519444444442</v>
+      </c>
+      <c r="O76" s="2">
+        <v>42817.552777777775</v>
+      </c>
+      <c r="P76" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>50</v>
+      </c>
+      <c r="R76" s="2">
+        <v>42817.638194444444</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="2">
+        <v>42814.367361111108</v>
+      </c>
+      <c r="D79" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79" s="2">
+        <v>42814.583333333336</v>
+      </c>
+      <c r="G79" s="2">
+        <v>42815.555555555555</v>
+      </c>
+      <c r="H79" t="s">
+        <v>54</v>
+      </c>
+      <c r="I79" t="s">
+        <v>50</v>
+      </c>
+      <c r="J79" s="2">
+        <v>42815.677777777775</v>
+      </c>
+      <c r="K79" s="2">
+        <v>42816.388888888891</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M79" t="s">
+        <v>50</v>
+      </c>
+      <c r="N79" s="2">
+        <v>42816.519444444442</v>
+      </c>
+      <c r="O79" s="2">
+        <v>42817.552777777775</v>
+      </c>
+      <c r="P79" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>50</v>
+      </c>
+      <c r="R79" s="2">
+        <v>42817.638194444444</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="2">
+        <v>42814.367361111108</v>
+      </c>
+      <c r="D82" t="s">
+        <v>51</v>
+      </c>
+      <c r="E82" t="s">
+        <v>50</v>
+      </c>
+      <c r="F82" s="2">
+        <v>42814.583333333336</v>
+      </c>
+      <c r="G82" s="2">
+        <v>42815.555555555555</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J82" s="2">
+        <v>42815.677777777775</v>
+      </c>
+      <c r="K82" s="2">
+        <v>42816.388888888891</v>
+      </c>
+      <c r="L82" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M82" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N82" s="2">
+        <v>42816.519444444442</v>
+      </c>
+      <c r="O82" s="2">
+        <v>42817.552777777775</v>
+      </c>
+      <c r="P82" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>50</v>
+      </c>
+      <c r="R82" s="2">
+        <v>42817.638194444444</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added 1gb database and logs to the project
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="66">
   <si>
     <t>vm1</t>
   </si>
@@ -208,6 +208,21 @@
   </si>
   <si>
     <t>147.25MB</t>
+  </si>
+  <si>
+    <t>270.25MB</t>
+  </si>
+  <si>
+    <t>952.25MB</t>
+  </si>
+  <si>
+    <t>1586.25MB</t>
+  </si>
+  <si>
+    <t>685.25MB</t>
+  </si>
+  <si>
+    <t>447.25MB</t>
   </si>
 </sst>
 </file>
@@ -1498,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70"/>
+    <sheetView tabSelected="1" topLeftCell="L46" workbookViewId="0">
+      <selection activeCell="S59" sqref="S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,9 +1535,16 @@
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="26.7109375" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1"/>
     <col min="17" max="17" width="16.7109375" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" customWidth="1"/>
+    <col min="19" max="19" width="19" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" customWidth="1"/>
+    <col min="22" max="22" width="23.85546875" customWidth="1"/>
+    <col min="23" max="23" width="23.5703125" customWidth="1"/>
+    <col min="24" max="24" width="13" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1998,47 +2020,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -2090,8 +2112,29 @@
       <c r="R75" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S75" t="s">
+        <v>47</v>
+      </c>
+      <c r="T75" t="s">
+        <v>46</v>
+      </c>
+      <c r="U75" t="s">
+        <v>48</v>
+      </c>
+      <c r="V75" t="s">
+        <v>52</v>
+      </c>
+      <c r="W75" t="s">
+        <v>47</v>
+      </c>
+      <c r="X75" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2143,13 +2186,34 @@
       <c r="R76" s="2">
         <v>42817.638194444444</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S76" s="2">
+        <v>42821.37222222222</v>
+      </c>
+      <c r="T76" t="s">
+        <v>62</v>
+      </c>
+      <c r="U76" t="s">
+        <v>50</v>
+      </c>
+      <c r="V76" s="2">
+        <v>42822.305555555555</v>
+      </c>
+      <c r="W76" s="2">
+        <v>42823.476388888892</v>
+      </c>
+      <c r="X76" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2201,13 +2265,34 @@
       <c r="R79" s="2">
         <v>42817.638194444444</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S79" s="2">
+        <v>42821.37222222222</v>
+      </c>
+      <c r="T79" t="s">
+        <v>61</v>
+      </c>
+      <c r="U79" t="s">
+        <v>50</v>
+      </c>
+      <c r="V79" s="2">
+        <v>42822.305555555555</v>
+      </c>
+      <c r="W79" s="2">
+        <v>42823.476388888892</v>
+      </c>
+      <c r="X79" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -2259,8 +2344,29 @@
       <c r="R82" s="2">
         <v>42817.638194444444</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S82" s="2">
+        <v>42821.37222222222</v>
+      </c>
+      <c r="T82" t="s">
+        <v>57</v>
+      </c>
+      <c r="U82" t="s">
+        <v>50</v>
+      </c>
+      <c r="V82" s="2">
+        <v>42822.305555555555</v>
+      </c>
+      <c r="W82" s="2">
+        <v>42823.476388888892</v>
+      </c>
+      <c r="X82" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>5</v>
       </c>

</xml_diff>